<commit_message>
latest updated data to investigate different response
</commit_message>
<xml_diff>
--- a/MicrocontrollerLab/Lab6/Raw_Bode_data_HDD_8k_sampling_Kp_7.xlsx
+++ b/MicrocontrollerLab/Lab6/Raw_Bode_data_HDD_8k_sampling_Kp_7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Control-Labs\MicrocontrollerLab\Lab6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8F9190B-8D20-4796-9DDE-AC05D2BB87EC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{574F8890-3C68-4A45-B6A1-D550FE2C387C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{455CE5E4-C782-4865-BC5A-EE0343CBF95E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
   <si>
     <t>freq</t>
   </si>
@@ -406,15 +406,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92127DDA-489C-47FC-A159-72B09E0D358C}">
-  <dimension ref="A1:AA30"/>
+  <dimension ref="A1:AO30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA2" sqref="AA2:AA25"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="AL15" sqref="AL15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -445,8 +445,23 @@
       <c r="T1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AF1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0.2</v>
       </c>
@@ -496,8 +511,34 @@
       <c r="AA2">
         <v>-5.76</v>
       </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AF2">
+        <v>0.8</v>
+      </c>
+      <c r="AG2">
+        <v>0.504</v>
+      </c>
+      <c r="AH2">
+        <v>0.52800000000000002</v>
+      </c>
+      <c r="AI2">
+        <v>0</v>
+      </c>
+      <c r="AJ2">
+        <f t="shared" ref="AJ2:AJ23" si="1">-AI2*10^-3*AF2*360</f>
+        <v>0</v>
+      </c>
+      <c r="AM2">
+        <v>0.8</v>
+      </c>
+      <c r="AN2">
+        <f>AH2/AG2</f>
+        <v>1.0476190476190477</v>
+      </c>
+      <c r="AO2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0.6</v>
       </c>
@@ -514,11 +555,11 @@
         <v>0.6</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K30" si="1">C3/B3</f>
+        <f t="shared" ref="K3:K30" si="2">C3/B3</f>
         <v>0.89423076923076927</v>
       </c>
       <c r="L3">
-        <f t="shared" ref="L3:L30" si="2">-1*D3</f>
+        <f t="shared" ref="L3:L30" si="3">-1*D3</f>
         <v>-4</v>
       </c>
       <c r="P3">
@@ -547,8 +588,34 @@
       <c r="AA3">
         <v>-9.2160000000000011</v>
       </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AF3">
+        <v>2</v>
+      </c>
+      <c r="AG3">
+        <v>0.504</v>
+      </c>
+      <c r="AH3">
+        <v>0.52800000000000002</v>
+      </c>
+      <c r="AI3">
+        <v>4</v>
+      </c>
+      <c r="AJ3">
+        <f>-AI3*10^-3*AF3*360</f>
+        <v>-2.88</v>
+      </c>
+      <c r="AM3">
+        <v>2</v>
+      </c>
+      <c r="AN3">
+        <f t="shared" ref="AN3:AN30" si="4">AH3/AG3</f>
+        <v>1.0476190476190477</v>
+      </c>
+      <c r="AO3">
+        <v>-2.88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.8</v>
       </c>
@@ -565,11 +632,11 @@
         <v>0.8</v>
       </c>
       <c r="K4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.93203883495145634</v>
       </c>
       <c r="L4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-5</v>
       </c>
       <c r="P4">
@@ -598,8 +665,34 @@
       <c r="AA4">
         <v>-8.0640000000000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AF4">
+        <v>4</v>
+      </c>
+      <c r="AG4">
+        <v>0.504</v>
+      </c>
+      <c r="AH4">
+        <v>0.53600000000000003</v>
+      </c>
+      <c r="AI4">
+        <v>4</v>
+      </c>
+      <c r="AJ4">
+        <f>-AI4*10^-3*AF4*360</f>
+        <v>-5.76</v>
+      </c>
+      <c r="AM4">
+        <v>4</v>
+      </c>
+      <c r="AN4">
+        <f t="shared" si="4"/>
+        <v>1.0634920634920635</v>
+      </c>
+      <c r="AO4">
+        <v>-5.76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -616,11 +709,11 @@
         <v>1</v>
       </c>
       <c r="K5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.88461538461538469</v>
       </c>
       <c r="L5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-7</v>
       </c>
       <c r="P5">
@@ -636,7 +729,7 @@
         <v>16</v>
       </c>
       <c r="T5">
-        <f t="shared" ref="T5:T22" si="3">-S5*10^-3*P5*360</f>
+        <f t="shared" ref="T5:T22" si="5">-S5*10^-3*P5*360</f>
         <v>-10.368</v>
       </c>
       <c r="Y5">
@@ -649,8 +742,34 @@
       <c r="AA5">
         <v>-10.368</v>
       </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AF5">
+        <v>8</v>
+      </c>
+      <c r="AG5">
+        <v>0.504</v>
+      </c>
+      <c r="AH5">
+        <v>0.55200000000000005</v>
+      </c>
+      <c r="AI5">
+        <v>4</v>
+      </c>
+      <c r="AJ5">
+        <f>-AI5*10^-3*AF5*360</f>
+        <v>-11.52</v>
+      </c>
+      <c r="AM5">
+        <v>8</v>
+      </c>
+      <c r="AN5">
+        <f t="shared" si="4"/>
+        <v>1.0952380952380953</v>
+      </c>
+      <c r="AO5">
+        <v>-11.52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1.2</v>
       </c>
@@ -667,11 +786,11 @@
         <v>1.2</v>
       </c>
       <c r="K6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.87378640776699035</v>
       </c>
       <c r="L6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-8</v>
       </c>
       <c r="P6">
@@ -687,7 +806,7 @@
         <v>20</v>
       </c>
       <c r="T6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-14.4</v>
       </c>
       <c r="Y6">
@@ -700,8 +819,34 @@
       <c r="AA6">
         <v>-14.4</v>
       </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AF6">
+        <v>13</v>
+      </c>
+      <c r="AG6">
+        <v>0.504</v>
+      </c>
+      <c r="AH6">
+        <v>0.61599999999999999</v>
+      </c>
+      <c r="AI6">
+        <v>3.2</v>
+      </c>
+      <c r="AJ6">
+        <f>-AI6*10^-3*AF6*360</f>
+        <v>-14.976000000000003</v>
+      </c>
+      <c r="AM6">
+        <v>13</v>
+      </c>
+      <c r="AN6">
+        <f t="shared" si="4"/>
+        <v>1.2222222222222221</v>
+      </c>
+      <c r="AO6">
+        <v>-14.976000000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1.4</v>
       </c>
@@ -718,11 +863,11 @@
         <v>1.4</v>
       </c>
       <c r="K7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.86538461538461542</v>
       </c>
       <c r="L7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-10</v>
       </c>
       <c r="P7">
@@ -738,7 +883,7 @@
         <v>20</v>
       </c>
       <c r="T7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-18.720000000000002</v>
       </c>
       <c r="Y7">
@@ -751,8 +896,34 @@
       <c r="AA7">
         <v>-18.720000000000002</v>
       </c>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AF7">
+        <v>17</v>
+      </c>
+      <c r="AG7">
+        <v>0.504</v>
+      </c>
+      <c r="AH7">
+        <v>0.68</v>
+      </c>
+      <c r="AI7">
+        <v>3.2</v>
+      </c>
+      <c r="AJ7">
+        <f>-AI7*10^-3*AF7*360</f>
+        <v>-19.584000000000003</v>
+      </c>
+      <c r="AM7">
+        <v>17</v>
+      </c>
+      <c r="AN7">
+        <f t="shared" si="4"/>
+        <v>1.3492063492063493</v>
+      </c>
+      <c r="AO7">
+        <v>-19.584000000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1.6</v>
       </c>
@@ -769,11 +940,11 @@
         <v>1.6</v>
       </c>
       <c r="K8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.89320388349514568</v>
       </c>
       <c r="L8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-13</v>
       </c>
       <c r="P8">
@@ -789,7 +960,7 @@
         <v>16</v>
       </c>
       <c r="T8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-18.432000000000002</v>
       </c>
       <c r="Y8">
@@ -802,8 +973,34 @@
       <c r="AA8">
         <v>-18.432000000000002</v>
       </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AF8">
+        <v>20</v>
+      </c>
+      <c r="AG8">
+        <v>0.50800000000000001</v>
+      </c>
+      <c r="AH8">
+        <v>0.752</v>
+      </c>
+      <c r="AI8">
+        <v>3.2</v>
+      </c>
+      <c r="AJ8">
+        <f>-AI8*10^-3*AF8*360</f>
+        <v>-23.04</v>
+      </c>
+      <c r="AM8">
+        <v>20</v>
+      </c>
+      <c r="AN8">
+        <f t="shared" si="4"/>
+        <v>1.4803149606299213</v>
+      </c>
+      <c r="AO8">
+        <v>-23.04</v>
+      </c>
+    </row>
+    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1.8</v>
       </c>
@@ -820,11 +1017,11 @@
         <v>1.8</v>
       </c>
       <c r="K9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.85576923076923073</v>
       </c>
       <c r="L9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-15</v>
       </c>
       <c r="P9">
@@ -840,7 +1037,7 @@
         <v>22</v>
       </c>
       <c r="T9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-31.68</v>
       </c>
       <c r="Y9">
@@ -853,8 +1050,34 @@
       <c r="AA9">
         <v>-31.68</v>
       </c>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AF9">
+        <v>21</v>
+      </c>
+      <c r="AG9">
+        <v>0.504</v>
+      </c>
+      <c r="AH9">
+        <v>0.78400000000000003</v>
+      </c>
+      <c r="AI9">
+        <v>3.2</v>
+      </c>
+      <c r="AJ9">
+        <f>-AI9*10^-3*AF9*360</f>
+        <v>-24.192000000000004</v>
+      </c>
+      <c r="AM9">
+        <v>21</v>
+      </c>
+      <c r="AN9">
+        <f t="shared" si="4"/>
+        <v>1.5555555555555556</v>
+      </c>
+      <c r="AO9">
+        <v>-24.192000000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2</v>
       </c>
@@ -871,11 +1094,11 @@
         <v>2</v>
       </c>
       <c r="K10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.84615384615384615</v>
       </c>
       <c r="L10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-22</v>
       </c>
       <c r="P10">
@@ -891,7 +1114,7 @@
         <v>14</v>
       </c>
       <c r="T10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-30.240000000000002</v>
       </c>
       <c r="Y10">
@@ -904,8 +1127,34 @@
       <c r="AA10">
         <v>-30.240000000000002</v>
       </c>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AF10">
+        <v>22</v>
+      </c>
+      <c r="AG10">
+        <v>0.504</v>
+      </c>
+      <c r="AH10">
+        <v>0.85599999999999998</v>
+      </c>
+      <c r="AI10">
+        <v>2.4</v>
+      </c>
+      <c r="AJ10">
+        <f>-AI10*10^-3*AF10*360</f>
+        <v>-19.007999999999999</v>
+      </c>
+      <c r="AM10">
+        <v>22</v>
+      </c>
+      <c r="AN10">
+        <f t="shared" si="4"/>
+        <v>1.6984126984126984</v>
+      </c>
+      <c r="AO10">
+        <v>-19.007999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2.2000000000000002</v>
       </c>
@@ -922,11 +1171,11 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="K11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.84615384615384615</v>
       </c>
       <c r="L11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-18</v>
       </c>
       <c r="P11">
@@ -942,7 +1191,7 @@
         <v>12.8</v>
       </c>
       <c r="T11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-36.864000000000004</v>
       </c>
       <c r="Y11">
@@ -955,8 +1204,34 @@
       <c r="AA11">
         <v>-36.864000000000004</v>
       </c>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AF11">
+        <v>23</v>
+      </c>
+      <c r="AG11">
+        <v>0.48799999999999999</v>
+      </c>
+      <c r="AH11">
+        <v>0.90400000000000003</v>
+      </c>
+      <c r="AI11">
+        <v>3.2</v>
+      </c>
+      <c r="AJ11">
+        <f>-AI11*10^-3*AF11*360</f>
+        <v>-26.495999999999999</v>
+      </c>
+      <c r="AM11">
+        <v>23</v>
+      </c>
+      <c r="AN11">
+        <f t="shared" si="4"/>
+        <v>1.8524590163934427</v>
+      </c>
+      <c r="AO11">
+        <v>-26.495999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2.4</v>
       </c>
@@ -973,11 +1248,11 @@
         <v>2.4</v>
       </c>
       <c r="K12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.89320388349514568</v>
       </c>
       <c r="L12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-17</v>
       </c>
       <c r="P12">
@@ -993,7 +1268,7 @@
         <v>13.6</v>
       </c>
       <c r="T12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-48.959999999999994</v>
       </c>
       <c r="Y12">
@@ -1006,8 +1281,34 @@
       <c r="AA12">
         <v>-48.959999999999994</v>
       </c>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AF12">
+        <v>25</v>
+      </c>
+      <c r="AG12">
+        <v>0.48</v>
+      </c>
+      <c r="AH12">
+        <v>0.92800000000000005</v>
+      </c>
+      <c r="AI12">
+        <v>4</v>
+      </c>
+      <c r="AJ12">
+        <f>-AI12*10^-3*AF12*360</f>
+        <v>-36</v>
+      </c>
+      <c r="AM12">
+        <v>25</v>
+      </c>
+      <c r="AN12">
+        <f t="shared" si="4"/>
+        <v>1.9333333333333336</v>
+      </c>
+      <c r="AO12">
+        <v>-36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2.6</v>
       </c>
@@ -1024,11 +1325,11 @@
         <v>2.6</v>
       </c>
       <c r="K13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.86407766990291268</v>
       </c>
       <c r="L13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-24</v>
       </c>
       <c r="P13">
@@ -1044,7 +1345,7 @@
         <v>15.2</v>
       </c>
       <c r="T13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-71.135999999999996</v>
       </c>
       <c r="Y13">
@@ -1057,8 +1358,34 @@
       <c r="AA13">
         <v>-71.135999999999996</v>
       </c>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AF13">
+        <v>27</v>
+      </c>
+      <c r="AG13">
+        <v>0.2</v>
+      </c>
+      <c r="AH13">
+        <v>0.42</v>
+      </c>
+      <c r="AI13">
+        <v>2.8</v>
+      </c>
+      <c r="AJ13">
+        <f>-AI13*10^-3*AF13*360</f>
+        <v>-27.216000000000001</v>
+      </c>
+      <c r="AM13">
+        <v>27</v>
+      </c>
+      <c r="AN13">
+        <f t="shared" si="4"/>
+        <v>2.0999999999999996</v>
+      </c>
+      <c r="AO13">
+        <v>-42.768000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2.8</v>
       </c>
@@ -1075,11 +1402,11 @@
         <v>2.8</v>
       </c>
       <c r="K14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.87378640776699035</v>
       </c>
       <c r="L14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-20</v>
       </c>
       <c r="P14">
@@ -1095,7 +1422,7 @@
         <v>16.399999999999999</v>
       </c>
       <c r="T14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-88.559999999999988</v>
       </c>
       <c r="Y14">
@@ -1108,8 +1435,34 @@
       <c r="AA14">
         <v>-88.559999999999988</v>
       </c>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AF14">
+        <v>30</v>
+      </c>
+      <c r="AG14">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="AH14">
+        <v>0.66400000000000003</v>
+      </c>
+      <c r="AI14">
+        <v>2.8</v>
+      </c>
+      <c r="AJ14">
+        <f>-AI14*10^-3*AF14*360</f>
+        <v>-30.240000000000002</v>
+      </c>
+      <c r="AM14">
+        <v>30</v>
+      </c>
+      <c r="AN14">
+        <f t="shared" si="4"/>
+        <v>2.3714285714285714</v>
+      </c>
+      <c r="AO14">
+        <v>-64.8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>3</v>
       </c>
@@ -1126,11 +1479,11 @@
         <v>3</v>
       </c>
       <c r="K15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.94174757281553401</v>
       </c>
       <c r="L15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-25</v>
       </c>
       <c r="P15">
@@ -1146,7 +1499,7 @@
         <v>17.2</v>
       </c>
       <c r="T15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-105.264</v>
       </c>
       <c r="Y15">
@@ -1159,8 +1512,34 @@
       <c r="AA15">
         <v>-105.264</v>
       </c>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AF15">
+        <v>31</v>
+      </c>
+      <c r="AG15">
+        <v>0.34399999999999997</v>
+      </c>
+      <c r="AH15">
+        <v>0.96799999999999997</v>
+      </c>
+      <c r="AI15">
+        <v>3.2</v>
+      </c>
+      <c r="AJ15">
+        <f>-AI15*10^-3*AF15*360</f>
+        <v>-35.712000000000003</v>
+      </c>
+      <c r="AM15">
+        <v>35</v>
+      </c>
+      <c r="AN15">
+        <f>AH17/AG17</f>
+        <v>3.7692307692307696</v>
+      </c>
+      <c r="AO15">
+        <v>-115.92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>4</v>
       </c>
@@ -1177,11 +1556,11 @@
         <v>4</v>
       </c>
       <c r="K16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.85576923076923073</v>
       </c>
       <c r="L16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-30</v>
       </c>
       <c r="P16">
@@ -1197,7 +1576,7 @@
         <v>17.2</v>
       </c>
       <c r="T16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-123.83999999999999</v>
       </c>
       <c r="Y16">
@@ -1210,8 +1589,34 @@
       <c r="AA16">
         <v>-123.83999999999999</v>
       </c>
-    </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AF16">
+        <v>33</v>
+      </c>
+      <c r="AG16">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="AH16">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="AI16">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="AJ16">
+        <f>-AI16*10^-3*AF16*360</f>
+        <v>-52.271999999999998</v>
+      </c>
+      <c r="AM16">
+        <v>37</v>
+      </c>
+      <c r="AN16">
+        <f>AH18/AG18</f>
+        <v>2.3055555555555558</v>
+      </c>
+      <c r="AO16">
+        <v>-133.19999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>5</v>
       </c>
@@ -1228,11 +1633,11 @@
         <v>5</v>
       </c>
       <c r="K17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.88461538461538469</v>
       </c>
       <c r="L17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-40</v>
       </c>
       <c r="P17">
@@ -1248,7 +1653,7 @@
         <v>17.600000000000001</v>
       </c>
       <c r="T17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-133.05600000000001</v>
       </c>
       <c r="Y17">
@@ -1261,8 +1666,34 @@
       <c r="AA17">
         <v>-133.05600000000001</v>
       </c>
-    </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AF17">
+        <v>35</v>
+      </c>
+      <c r="AG17">
+        <v>0.20799999999999999</v>
+      </c>
+      <c r="AH17">
+        <v>0.78400000000000003</v>
+      </c>
+      <c r="AI17">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="AJ17">
+        <f>-AI17*10^-3*AF17*360</f>
+        <v>-115.92</v>
+      </c>
+      <c r="AM17">
+        <v>40</v>
+      </c>
+      <c r="AN17">
+        <f>AH19/AG19</f>
+        <v>1.7777777777777779</v>
+      </c>
+      <c r="AO17">
+        <v>-144</v>
+      </c>
+    </row>
+    <row r="18" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>6</v>
       </c>
@@ -1279,11 +1710,11 @@
         <v>6</v>
       </c>
       <c r="K18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.86904761904761907</v>
       </c>
       <c r="L18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-52</v>
       </c>
       <c r="P18">
@@ -1299,7 +1730,7 @@
         <v>16.8</v>
       </c>
       <c r="T18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-151.20000000000002</v>
       </c>
       <c r="Y18">
@@ -1312,8 +1743,34 @@
       <c r="AA18">
         <v>-151.20000000000002</v>
       </c>
-    </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AF18">
+        <v>37</v>
+      </c>
+      <c r="AG18">
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="AH18">
+        <v>0.66400000000000003</v>
+      </c>
+      <c r="AI18">
+        <v>10</v>
+      </c>
+      <c r="AJ18">
+        <f>-AI18*10^-3*AF18*360</f>
+        <v>-133.19999999999999</v>
+      </c>
+      <c r="AM18">
+        <v>42</v>
+      </c>
+      <c r="AN18">
+        <f>AH20/AG20</f>
+        <v>1.3333333333333335</v>
+      </c>
+      <c r="AO18">
+        <v>-157.24800000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>7</v>
       </c>
@@ -1330,11 +1787,11 @@
         <v>7</v>
       </c>
       <c r="K19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.82692307692307687</v>
       </c>
       <c r="L19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-55</v>
       </c>
       <c r="P19">
@@ -1350,7 +1807,7 @@
         <v>16</v>
       </c>
       <c r="T19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-155.52000000000001</v>
       </c>
       <c r="Y19">
@@ -1363,8 +1820,34 @@
       <c r="AA19">
         <v>-155.52000000000001</v>
       </c>
-    </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AF19">
+        <v>40</v>
+      </c>
+      <c r="AG19">
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="AH19">
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="AI19">
+        <v>10</v>
+      </c>
+      <c r="AJ19">
+        <f>-AI19*10^-3*AF19*360</f>
+        <v>-144</v>
+      </c>
+      <c r="AM19">
+        <v>45</v>
+      </c>
+      <c r="AN19">
+        <f>AH21/AG21</f>
+        <v>1.0634920634920635</v>
+      </c>
+      <c r="AO19">
+        <v>-162</v>
+      </c>
+    </row>
+    <row r="20" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>8</v>
       </c>
@@ -1381,11 +1864,11 @@
         <v>8</v>
       </c>
       <c r="K20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.81310679611650494</v>
       </c>
       <c r="L20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-63</v>
       </c>
       <c r="P20">
@@ -1401,7 +1884,7 @@
         <v>15.2</v>
       </c>
       <c r="T20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-164.16</v>
       </c>
       <c r="Y20">
@@ -1414,8 +1897,34 @@
       <c r="AA20">
         <v>-164.16</v>
       </c>
-    </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AF20">
+        <v>42</v>
+      </c>
+      <c r="AG20">
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="AH20">
+        <v>0.38400000000000001</v>
+      </c>
+      <c r="AI20">
+        <v>10.4</v>
+      </c>
+      <c r="AJ20">
+        <f>-AI20*10^-3*AF20*360</f>
+        <v>-157.24800000000002</v>
+      </c>
+      <c r="AM20">
+        <v>50</v>
+      </c>
+      <c r="AN20">
+        <f>AH22/AG22</f>
+        <v>0.96825396825396826</v>
+      </c>
+      <c r="AO20">
+        <v>-165.6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>9</v>
       </c>
@@ -1432,11 +1941,11 @@
         <v>9</v>
       </c>
       <c r="K21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.74038461538461542</v>
       </c>
       <c r="L21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-80</v>
       </c>
       <c r="P21">
@@ -1452,7 +1961,7 @@
         <v>13.6</v>
       </c>
       <c r="T21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-171.35999999999999</v>
       </c>
       <c r="Y21">
@@ -1465,8 +1974,34 @@
       <c r="AA21">
         <v>-171.35999999999999</v>
       </c>
-    </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AF21">
+        <v>45</v>
+      </c>
+      <c r="AG21">
+        <v>0.504</v>
+      </c>
+      <c r="AH21">
+        <v>0.53600000000000003</v>
+      </c>
+      <c r="AI21">
+        <v>10</v>
+      </c>
+      <c r="AJ21">
+        <f>-AI21*10^-3*AF21*360</f>
+        <v>-162</v>
+      </c>
+      <c r="AM21">
+        <v>55</v>
+      </c>
+      <c r="AN21">
+        <f>AH23/AG23</f>
+        <v>0.66666666666666674</v>
+      </c>
+      <c r="AO21">
+        <v>-174.24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>10</v>
       </c>
@@ -1483,11 +2018,11 @@
         <v>10</v>
       </c>
       <c r="K22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.68269230769230771</v>
       </c>
       <c r="L22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-90</v>
       </c>
       <c r="P22">
@@ -1503,7 +2038,7 @@
         <v>13.2</v>
       </c>
       <c r="T22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-175.82400000000001</v>
       </c>
       <c r="Y22">
@@ -1516,8 +2051,34 @@
       <c r="AA22">
         <v>-175.82400000000001</v>
       </c>
-    </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AF22">
+        <v>50</v>
+      </c>
+      <c r="AG22">
+        <v>0.504</v>
+      </c>
+      <c r="AH22">
+        <v>0.48799999999999999</v>
+      </c>
+      <c r="AI22">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="AJ22">
+        <f>-AI22*10^-3*AF22*360</f>
+        <v>-165.6</v>
+      </c>
+      <c r="AM22">
+        <v>60</v>
+      </c>
+      <c r="AN22">
+        <f>AH24/AG24</f>
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="AO22">
+        <v>-181.44000000000005</v>
+      </c>
+    </row>
+    <row r="23" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>11</v>
       </c>
@@ -1534,11 +2095,11 @@
         <v>11</v>
       </c>
       <c r="K23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.625</v>
       </c>
       <c r="L23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-101</v>
       </c>
       <c r="P23">
@@ -1567,8 +2128,34 @@
       <c r="AA23">
         <v>-184.32</v>
       </c>
-    </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AF23">
+        <v>55</v>
+      </c>
+      <c r="AG23">
+        <v>0.504</v>
+      </c>
+      <c r="AH23">
+        <v>0.33600000000000002</v>
+      </c>
+      <c r="AI23">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="AJ23">
+        <f>-AI23*10^-3*AF23*360</f>
+        <v>-174.24</v>
+      </c>
+      <c r="AM23">
+        <v>65</v>
+      </c>
+      <c r="AN23">
+        <f>AH25/AG25</f>
+        <v>0.4296875</v>
+      </c>
+      <c r="AO23">
+        <v>-196.56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>13</v>
       </c>
@@ -1585,11 +2172,11 @@
         <v>13</v>
       </c>
       <c r="K24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.58252427184466016</v>
       </c>
       <c r="L24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-120</v>
       </c>
       <c r="P24">
@@ -1618,8 +2205,24 @@
       <c r="AA24">
         <v>-181.44</v>
       </c>
-    </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AF24">
+        <v>60</v>
+      </c>
+      <c r="AG24">
+        <v>0.504</v>
+      </c>
+      <c r="AH24">
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="AI24">
+        <v>8.4</v>
+      </c>
+      <c r="AJ24">
+        <f>-AI24*10^-3*AF24*360</f>
+        <v>-181.44000000000005</v>
+      </c>
+    </row>
+    <row r="25" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>15</v>
       </c>
@@ -1636,11 +2239,11 @@
         <v>15</v>
       </c>
       <c r="K25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.41346153846153844</v>
       </c>
       <c r="L25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-130</v>
       </c>
       <c r="P25">
@@ -1669,8 +2272,24 @@
       <c r="AA25">
         <v>-187.92000000000002</v>
       </c>
-    </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AF25">
+        <v>65</v>
+      </c>
+      <c r="AG25">
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="AH25">
+        <v>0.22</v>
+      </c>
+      <c r="AI25">
+        <v>8.4</v>
+      </c>
+      <c r="AJ25">
+        <f>-AI25*10^-3*AF25*360</f>
+        <v>-196.56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>17</v>
       </c>
@@ -1687,15 +2306,15 @@
         <v>17</v>
       </c>
       <c r="K26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.36407766990291263</v>
       </c>
       <c r="L26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-137</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>19</v>
       </c>
@@ -1712,15 +2331,15 @@
         <v>19</v>
       </c>
       <c r="K27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.2718446601941748</v>
       </c>
       <c r="L27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-132</v>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>21</v>
       </c>
@@ -1737,15 +2356,15 @@
         <v>21</v>
       </c>
       <c r="K28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.22815533980582525</v>
       </c>
       <c r="L28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-140</v>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>25</v>
       </c>
@@ -1762,15 +2381,15 @@
         <v>25</v>
       </c>
       <c r="K29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.18446601941747573</v>
       </c>
       <c r="L29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-170</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>27</v>
       </c>
@@ -1787,11 +2406,11 @@
         <v>27</v>
       </c>
       <c r="K30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.16747572815533984</v>
       </c>
       <c r="L30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-180</v>
       </c>
     </row>

</xml_diff>